<commit_message>
add parameter file check
</commit_message>
<xml_diff>
--- a/parameter_template.xlsx
+++ b/parameter_template.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LIMIANHUANG\workspace\download-report\dlr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mohan\Code\Git\dlr\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="6060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6060"/>
   </bookViews>
   <sheets>
     <sheet name="request" sheetId="1" r:id="rId1"/>
     <sheet name="parameter" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
     <definedName name="编辑1." localSheetId="1">parameter!$A$1:$B$33</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="85">
   <si>
     <t>Select Report Level</t>
   </si>
@@ -290,17 +293,21 @@
   </si>
   <si>
     <t>Input Field</t>
+  </si>
+  <si>
+    <t>Employee</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -308,15 +315,22 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -407,6 +421,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="request"/>
+      <sheetName val="parameter"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -711,24 +740,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="17.125" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="13.625" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="45.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,7 +783,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="29.25" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -780,9 +809,185 @@
         <v>37</v>
       </c>
     </row>
+    <row r="3" spans="1:8" ht="29.25" thickBot="1">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="5">
+        <v>42728</v>
+      </c>
+      <c r="D3" s="5">
+        <v>43019</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="29.25" thickBot="1">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5">
+        <v>43019</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="29.25" thickBot="1">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="5">
+        <v>42728</v>
+      </c>
+      <c r="D5" s="5">
+        <v>43019</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="29.25" thickBot="1">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5">
+        <v>42728</v>
+      </c>
+      <c r="D6" s="5">
+        <v>43019</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="29.25" thickBot="1">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="5">
+        <v>42728</v>
+      </c>
+      <c r="D7" s="5">
+        <v>43019</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1"/>
+    <row r="10" spans="1:8" ht="29.25" thickBot="1">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5">
+        <v>42728</v>
+      </c>
+      <c r="D10" s="5">
+        <v>43019</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="29.25" thickBot="1">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="5">
+        <v>42728</v>
+      </c>
+      <c r="D11" s="5">
+        <v>43019</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D2">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D7 C10:D11">
       <formula1>40179</formula1>
       <formula2>72686</formula2>
     </dataValidation>
@@ -791,7 +996,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>parameter!$B$1:$B$2</xm:f>
@@ -822,6 +1027,36 @@
           </x14:formula1>
           <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]parameter!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3:B7 B10:B11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]parameter!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>G3:G7 G10:G11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]parameter!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3:F7 F10:F11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]parameter!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E7 E10:E11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]parameter!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>A3:A7 A10:A11</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -837,19 +1072,19 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="80.33203125" customWidth="1"/>
+    <col min="6" max="6" width="80.375" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -881,7 +1116,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -913,7 +1148,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="C3" t="s">
         <v>76</v>
       </c>
@@ -933,7 +1168,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="C4" t="s">
         <v>77</v>
       </c>
@@ -953,7 +1188,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="C5" t="s">
         <v>78</v>
       </c>
@@ -973,7 +1208,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="E6" t="s">
         <v>43</v>
       </c>
@@ -987,7 +1222,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="E7" t="s">
         <v>47</v>
       </c>
@@ -1001,7 +1236,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="E8" t="s">
         <v>46</v>
       </c>
@@ -1015,7 +1250,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="E9" t="s">
         <v>45</v>
       </c>
@@ -1029,7 +1264,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="E10" t="s">
         <v>55</v>
       </c>
@@ -1043,7 +1278,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="E11" t="s">
         <v>54</v>
       </c>
@@ -1057,7 +1292,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="E12" t="s">
         <v>49</v>
       </c>
@@ -1071,7 +1306,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="E13" t="s">
         <v>48</v>
       </c>
@@ -1079,7 +1314,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="E14" t="s">
         <v>53</v>
       </c>
@@ -1087,7 +1322,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="E15" t="s">
         <v>52</v>
       </c>
@@ -1095,7 +1330,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="E16" t="s">
         <v>51</v>
       </c>
@@ -1103,7 +1338,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:6">
       <c r="E17" t="s">
         <v>50</v>
       </c>
@@ -1112,6 +1347,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>